<commit_message>
fruit card stats updated
</commit_message>
<xml_diff>
--- a/Pre-GDC-prototype-addiction/Assets/docs/Fruit_card_stats.xlsx
+++ b/Pre-GDC-prototype-addiction/Assets/docs/Fruit_card_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Pre-GDC\Pre-GDC-prototype-addiction\Assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EB51A2-A171-42F6-97FC-875214DC2532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89A1EFC-B50C-4292-8393-BE08D9DB77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -528,10 +528,11 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <f>B2*3</f>
+        <v>300</v>
       </c>
       <c r="D2">
         <v>0.7</v>
@@ -540,54 +541,54 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G2">
         <f>B2*1.2</f>
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="H2">
         <v>0.3</v>
       </c>
       <c r="I2">
         <f>B2*2</f>
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="J2">
         <v>0.15</v>
       </c>
       <c r="K2">
         <f>B2*4</f>
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="L2">
-        <v>4.7E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="M2">
         <f>B2*25</f>
-        <v>250</v>
+        <v>2500</v>
       </c>
       <c r="N2">
         <v>2E-3</v>
       </c>
       <c r="O2">
         <f>B2*50</f>
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="P2">
         <v>1E-3</v>
       </c>
       <c r="R2">
         <f>G2*H2+I2*J2+K2*L2+M2*N2+O2*P2</f>
-        <v>9.48</v>
+        <v>134.80000000000001</v>
       </c>
       <c r="S2" s="4">
         <f>0.5*0.5*0.2*(0.7*(G2+I2+K2+M2+O2)+0.3*((G2*H2+K2*L2+M2*N2+O2*P2)/(1-J2)+(G2*H2+I2*J2+M2*N2+O2*P2)/(1-L2)+(G2*H2+I2*J2+K2*L2+O2*P2)/(1-N2)+(G2*H2+I2*J2+K2*L2+M2*N2)/(1-P2)))</f>
-        <v>29.273779961431462</v>
+        <v>294.78572207177552</v>
       </c>
       <c r="T2">
         <f>0.75*R2+0.25*S2</f>
-        <v>14.428444990357866</v>
+        <v>174.79643051794389</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -595,10 +596,11 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C3">
-        <v>150</v>
+        <f t="shared" ref="C3:C6" si="0">B3*3</f>
+        <v>600</v>
       </c>
       <c r="D3">
         <v>0.7</v>
@@ -607,54 +609,54 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G6" si="0">B3*1.2</f>
-        <v>60</v>
+        <f t="shared" ref="G3:G6" si="1">B3*1.2</f>
+        <v>240</v>
       </c>
       <c r="H3">
         <v>0.3</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I6" si="1">B3*2</f>
-        <v>100</v>
+        <f t="shared" ref="I3:I6" si="2">B3*2</f>
+        <v>400</v>
       </c>
       <c r="J3">
         <v>0.15</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K6" si="2">B3*5</f>
-        <v>250</v>
+        <f t="shared" ref="K3:K6" si="3">B3*5</f>
+        <v>1000</v>
       </c>
       <c r="L3">
-        <v>4.7E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M6" si="3">B3*25</f>
-        <v>1250</v>
+        <f t="shared" ref="M3:M6" si="4">B3*25</f>
+        <v>5000</v>
       </c>
       <c r="N3">
         <v>2E-3</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O6" si="4">B3*50</f>
-        <v>2500</v>
+        <f t="shared" ref="O3:O6" si="5">B3*50</f>
+        <v>10000</v>
       </c>
       <c r="P3">
         <v>1E-3</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R6" si="5">G3*H3+I3*J3+K3*L3+M3*N3+O3*P3</f>
-        <v>49.75</v>
+        <f t="shared" ref="R3:R6" si="6">G3*H3+I3*J3+K3*L3+M3*N3+O3*P3</f>
+        <v>299</v>
       </c>
       <c r="S3" s="4">
-        <f t="shared" ref="S3:S6" si="6">0.5*0.5*0.2*(0.7*(G3+I3+K3+M3+O3)+0.3*((G3*H3+K3*L3+M3*N3+O3*P3)/(1-J3)+(G3*H3+I3*J3+M3*N3+O3*P3)/(1-L3)+(G3*H3+I3*J3+K3*L3+O3*P3)/(1-N3)+(G3*H3+I3*J3+K3*L3+M3*N3)/(1-P3)))</f>
-        <v>148.23097632196047</v>
+        <f t="shared" ref="S3:S6" si="7">0.5*0.5*0.2*(0.7*(G3+I3+K3+M3+O3)+0.3*((G3*H3+K3*L3+M3*N3+O3*P3)/(1-J3)+(G3*H3+I3*J3+M3*N3+O3*P3)/(1-L3)+(G3*H3+I3*J3+K3*L3+O3*P3)/(1-N3)+(G3*H3+I3*J3+K3*L3+M3*N3)/(1-P3)))</f>
+        <v>597.97359288193934</v>
       </c>
       <c r="T3">
         <f>0.75*R3+0.25*S3</f>
-        <v>74.370244080490124</v>
+        <v>373.74339822048483</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -662,10 +664,11 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="C4">
-        <v>750</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="D4">
         <v>0.7</v>
@@ -674,54 +677,54 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f t="shared" si="1"/>
+        <v>600</v>
       </c>
       <c r="H4">
         <v>0.3</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <f t="shared" si="2"/>
+        <v>1000</v>
       </c>
       <c r="J4">
         <v>0.15</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
-        <v>1250</v>
+        <f t="shared" si="3"/>
+        <v>2500</v>
       </c>
       <c r="L4">
-        <v>4.7E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="M4">
-        <f t="shared" si="3"/>
-        <v>6250</v>
+        <f t="shared" si="4"/>
+        <v>12500</v>
       </c>
       <c r="N4">
         <v>2E-3</v>
       </c>
       <c r="O4">
-        <f t="shared" si="4"/>
-        <v>12500</v>
+        <f t="shared" si="5"/>
+        <v>25000</v>
       </c>
       <c r="P4">
         <v>1E-3</v>
       </c>
       <c r="R4">
-        <f t="shared" si="5"/>
-        <v>248.75</v>
+        <f t="shared" si="6"/>
+        <v>747.5</v>
       </c>
       <c r="S4" s="4">
-        <f t="shared" si="6"/>
-        <v>741.15488160980226</v>
+        <f t="shared" si="7"/>
+        <v>1494.9339822048482</v>
       </c>
       <c r="T4">
         <f>0.75*R4+0.25*S4</f>
-        <v>371.85122040245056</v>
+        <v>934.35849555121206</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -729,10 +732,11 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C5">
-        <v>3000</v>
+        <f t="shared" si="0"/>
+        <v>7500</v>
       </c>
       <c r="D5">
         <v>0.7</v>
@@ -741,54 +745,54 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>1200</v>
+        <f t="shared" si="1"/>
+        <v>3000</v>
       </c>
       <c r="H5">
         <v>0.3</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>2000</v>
+        <f t="shared" si="2"/>
+        <v>5000</v>
       </c>
       <c r="J5">
         <v>0.15</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>5000</v>
+        <f t="shared" si="3"/>
+        <v>12500</v>
       </c>
       <c r="L5">
-        <v>4.7E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="M5">
-        <f t="shared" si="3"/>
-        <v>25000</v>
+        <f t="shared" si="4"/>
+        <v>62500</v>
       </c>
       <c r="N5">
         <v>2E-3</v>
       </c>
       <c r="O5">
-        <f t="shared" si="4"/>
-        <v>50000</v>
+        <f t="shared" si="5"/>
+        <v>125000</v>
       </c>
       <c r="P5">
         <v>1E-3</v>
       </c>
       <c r="R5">
-        <f t="shared" si="5"/>
-        <v>995</v>
+        <f t="shared" si="6"/>
+        <v>3737.5</v>
       </c>
       <c r="S5" s="4">
-        <f t="shared" si="6"/>
-        <v>2964.619526439209</v>
+        <f t="shared" si="7"/>
+        <v>7474.6699110242425</v>
       </c>
       <c r="T5">
         <f>0.75*R5+0.25*S5</f>
-        <v>1487.4048816098023</v>
+        <v>4671.7924777560602</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -799,7 +803,8 @@
         <v>10000</v>
       </c>
       <c r="C6">
-        <v>100000</v>
+        <f t="shared" si="0"/>
+        <v>30000</v>
       </c>
       <c r="D6">
         <v>0.7</v>
@@ -808,54 +813,54 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12000</v>
       </c>
       <c r="H6">
         <v>0.3</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="J6">
         <v>0.15</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50000</v>
       </c>
       <c r="L6">
-        <v>4.7E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="M6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250000</v>
       </c>
       <c r="N6">
         <v>2E-3</v>
       </c>
       <c r="O6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>500000</v>
       </c>
       <c r="P6">
         <v>1E-3</v>
       </c>
       <c r="R6">
-        <f t="shared" si="5"/>
-        <v>9950</v>
+        <f t="shared" si="6"/>
+        <v>14950</v>
       </c>
       <c r="S6" s="4">
-        <f t="shared" si="6"/>
-        <v>29646.195264392092</v>
+        <f t="shared" si="7"/>
+        <v>29898.67964409697</v>
       </c>
       <c r="T6">
         <f>0.75*R6+0.25*S6</f>
-        <v>14874.048816098024</v>
+        <v>18687.169911024241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>